<commit_message>
Added shiny app and updated data
gl hf ;)
</commit_message>
<xml_diff>
--- a/Worklog.xlsx
+++ b/Worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sniss\OneDrive\Desktop\CSC 324\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FD8586A-2E8A-481E-9DB8-F92CD7090991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382157C8-737C-47E4-ABBB-E917DCEBE654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{778DB95B-FF96-4844-8E9A-163DE1662BC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{778DB95B-FF96-4844-8E9A-163DE1662BC6}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="13" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3147" uniqueCount="111">
   <si>
     <t>JANUARY  2022</t>
   </si>
@@ -13086,8 +13086,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13776,27 +13776,27 @@
       </c>
       <c r="B22" s="80"/>
       <c r="C22" s="85" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="D22" s="86"/>
       <c r="E22" s="85" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="F22" s="86"/>
       <c r="G22" s="85" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="H22" s="86"/>
       <c r="I22" s="85" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="J22" s="86"/>
       <c r="K22" s="85" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="L22" s="86"/>
       <c r="M22" s="79" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="N22" s="80"/>
     </row>
@@ -13806,15 +13806,13 @@
       </c>
       <c r="B23" s="80"/>
       <c r="C23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D23" s="86"/>
-      <c r="E23" s="85" t="s">
-        <v>8</v>
-      </c>
+      <c r="E23" s="85"/>
       <c r="F23" s="86"/>
       <c r="G23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H23" s="86"/>
       <c r="I23" s="85" t="s">
@@ -13822,7 +13820,7 @@
       </c>
       <c r="J23" s="86"/>
       <c r="K23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="L23" s="86"/>
       <c r="M23" s="79" t="s">
@@ -14030,7 +14028,7 @@
       </c>
       <c r="B30" s="80"/>
       <c r="C30" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D30" s="86"/>
       <c r="E30" s="81" t="s">
@@ -14481,8 +14479,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14639,7 +14637,7 @@
       </c>
       <c r="F5" s="86"/>
       <c r="G5" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H5" s="86"/>
       <c r="I5" s="85" t="s">
@@ -14647,7 +14645,7 @@
       </c>
       <c r="J5" s="86"/>
       <c r="K5" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="L5" s="86"/>
       <c r="M5" s="79" t="s">
@@ -14825,7 +14823,7 @@
       </c>
       <c r="B11" s="80"/>
       <c r="C11" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D11" s="86"/>
       <c r="E11" s="85" t="s">
@@ -14833,7 +14831,7 @@
       </c>
       <c r="F11" s="86"/>
       <c r="G11" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H11" s="86"/>
       <c r="I11" s="85" t="s">
@@ -14841,7 +14839,7 @@
       </c>
       <c r="J11" s="86"/>
       <c r="K11" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="L11" s="86"/>
       <c r="M11" s="79" t="s">
@@ -15019,7 +15017,7 @@
       </c>
       <c r="B17" s="80"/>
       <c r="C17" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D17" s="86"/>
       <c r="E17" s="85" t="s">
@@ -15027,15 +15025,13 @@
       </c>
       <c r="F17" s="86"/>
       <c r="G17" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H17" s="86"/>
-      <c r="I17" s="85" t="s">
-        <v>8</v>
-      </c>
+      <c r="I17" s="85"/>
       <c r="J17" s="86"/>
       <c r="K17" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="L17" s="86"/>
       <c r="M17" s="79" t="s">
@@ -15213,7 +15209,7 @@
       </c>
       <c r="B23" s="80"/>
       <c r="C23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D23" s="86"/>
       <c r="E23" s="85" t="s">
@@ -15221,7 +15217,7 @@
       </c>
       <c r="F23" s="86"/>
       <c r="G23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H23" s="86"/>
       <c r="I23" s="85" t="s">
@@ -15229,7 +15225,7 @@
       </c>
       <c r="J23" s="86"/>
       <c r="K23" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="L23" s="86"/>
       <c r="M23" s="79" t="s">
@@ -15407,7 +15403,7 @@
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D29" s="86"/>
       <c r="E29" s="85" t="s">
@@ -15415,7 +15411,7 @@
       </c>
       <c r="F29" s="86"/>
       <c r="G29" s="85" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H29" s="86"/>
       <c r="I29" s="85" t="s">

</xml_diff>